<commit_message>
WebDriverManager is added instead of the driver path
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaradhyaVashisht\git\SeleniumLearning\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA742109-35FD-44EE-9A38-F2F8978F56B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72672123-8990-4D8A-AF0E-78A2D89EADF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FF4E79BB-B70B-4CB5-A71B-57A09E3C6633}"/>
   </bookViews>
@@ -608,7 +608,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Latest excel changes are added for all testcases
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaradhyaVashisht\git\SeleniumLearning\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72672123-8990-4D8A-AF0E-78A2D89EADF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FF4E79BB-B70B-4CB5-A71B-57A09E3C6633}"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16590" windowHeight="2985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DemoWebShop" sheetId="1" r:id="rId1"/>
     <sheet name="OrangeHRM" sheetId="2" r:id="rId2"/>
     <sheet name="airbnb" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>TC No</t>
   </si>
@@ -130,9 +125,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Blood Group</t>
-  </si>
-  <si>
     <t>Message</t>
   </si>
   <si>
@@ -164,12 +156,33 @@
   </si>
   <si>
     <t>Australian</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Region-2</t>
+  </si>
+  <si>
+    <t>FTE</t>
+  </si>
+  <si>
+    <t>Temporary Department</t>
+  </si>
+  <si>
+    <t>Sub unit-3</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -214,10 +227,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -279,7 +300,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -331,7 +352,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -525,26 +546,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC8063E-A986-4827-AC0B-730F7574F51B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -594,207 +615,289 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{91424C15-7EAD-4F63-9639-7FD7298B9B5E}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{A12D04B7-2327-4218-8B55-942C09E7271E}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{CB349D4B-89FB-41D6-BD32-B2C8EF97F67C}"/>
-    <hyperlink ref="D3" r:id="rId4" xr:uid="{D458C343-023D-4A94-91E9-C564112BDAED}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{120B6CD2-16AA-49CB-AC76-0D8921D2611D}">
-  <dimension ref="A1:M7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M1" t="s">
-        <v>41</v>
+      <c r="M2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" t="s">
-        <v>42</v>
-      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="automation.catalogue@gmail.com" xr:uid="{5FDB84C1-13D1-41A3-8B6E-9934E87A29D7}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{C50C0E9D-606A-4472-BCE7-4261131B2E89}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{31DEFC17-2A19-4D70-8159-D2910B895881}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{AB6EF740-AB46-4B35-9C19-7D62F8A7B353}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{D042B2B0-E5F3-4F1E-8DBF-FF78758E523B}"/>
-    <hyperlink ref="C2" r:id="rId6" display="automation.catalogue@gmail.com" xr:uid="{4FCC12AF-BA84-4FFC-A72E-2B8D7DA01050}"/>
-    <hyperlink ref="D2" r:id="rId7" xr:uid="{25D05F66-9F19-45BC-A576-FD295EFA6220}"/>
+    <hyperlink ref="C3" r:id="rId1" display="automation.catalogue@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D7" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId6" display="automation.catalogue@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7E8728-91A6-44FD-8F68-6210EEB1F1D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest TestNG changes are included
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{968074F3-E32B-4DCE-ABB7-91D0FC15FB3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9687D13E-8C51-46AB-8A03-1A9EB7B7FFB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="16620" windowHeight="4428" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="16644" windowHeight="7836" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DemoWebShop" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="airbnb" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:O6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>TC No</t>
   </si>
@@ -43,15 +43,9 @@
     <t>DemoWebShop Login</t>
   </si>
   <si>
-    <t>aarosagarch@gmail.com</t>
-  </si>
-  <si>
     <t>Admin@123</t>
   </si>
   <si>
-    <t>automation.catalogue@gmail.com</t>
-  </si>
-  <si>
     <t>Test@1234</t>
   </si>
   <si>
@@ -173,6 +167,15 @@
   </si>
   <si>
     <t>0.5</t>
+  </si>
+  <si>
+    <t>log-in123@gmail.com</t>
+  </si>
+  <si>
+    <t>login@123</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -235,6 +238,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -296,7 +300,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -348,7 +352,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -552,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,7 +576,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -582,40 +586,30 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -624,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
@@ -659,99 +653,99 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="N1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="P1" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="M2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -768,16 +762,16 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -794,19 +788,19 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -822,16 +816,16 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -848,16 +842,16 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>

</xml_diff>

<commit_message>
new test case 02
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaradhyaVashisht\git\SeleniumLearning\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rehan\git\SeleniumLearning\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF5B7B6-D7C5-4E26-ADB1-D374595878E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA432308-98FF-46BA-8C1E-719DD406DAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t>TC No</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>Sagar</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -180,6 +177,15 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>aaliyah.haq</t>
   </si>
 </sst>
 </file>
@@ -580,7 +586,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -591,21 +597,21 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -620,10 +626,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,7 +646,7 @@
     <col min="16" max="16" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -657,42 +663,45 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>44</v>
+      <c r="Q1" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -704,49 +713,52 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="K2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
@@ -763,19 +775,22 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
+      <c r="Q3" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -790,21 +805,21 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -818,18 +833,18 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -844,18 +859,18 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -873,15 +888,15 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="automation.catalogue@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="C2" r:id="rId6" display="automation.catalogue@gmail.com" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="D2" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="C2" r:id="rId5" display="automation.catalogue@gmail.com" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="D2" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Allorderstotal test case updated
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaradhyaVashisht\git\SeleniumLearning\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rehan\git\SeleniumLearning\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CDC7CA-41A3-4B01-B37F-2770BEF62E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD79E36A-844A-4597-A3FD-5C59AB24F7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRMLogin" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>TC No</t>
   </si>
@@ -81,18 +81,9 @@
     <t>Vijetha</t>
   </si>
   <si>
-    <t>abcd!123</t>
-  </si>
-  <si>
-    <t>Prashanth</t>
-  </si>
-  <si>
     <t>Admin@1234</t>
   </si>
   <si>
-    <t>Sai</t>
-  </si>
-  <si>
     <t>Hello@1235</t>
   </si>
   <si>
@@ -171,61 +162,79 @@
     <t>0.5</t>
   </si>
   <si>
+    <t>login@123</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>aaliyah.haq</t>
+  </si>
+  <si>
+    <t>aarosagarch@gmail.com</t>
+  </si>
+  <si>
+    <t>Order number</t>
+  </si>
+  <si>
+    <t>997040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firstname </t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>Shane</t>
+  </si>
+  <si>
+    <t>Ward</t>
+  </si>
+  <si>
+    <t>TC_00_Login_OrangeHRM</t>
+  </si>
+  <si>
+    <t>Sagar</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>Demo123</t>
+  </si>
+  <si>
+    <t>Test456</t>
+  </si>
+  <si>
+    <t>log-in1234@gmail.com</t>
+  </si>
+  <si>
     <t>log-in123@gmail.com</t>
   </si>
   <si>
-    <t>login@123</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>options</t>
-  </si>
-  <si>
-    <t>Logout</t>
-  </si>
-  <si>
-    <t>aaliyah.haq</t>
-  </si>
-  <si>
-    <t>aarosagarch@gmail.com</t>
-  </si>
-  <si>
-    <t>Order number</t>
-  </si>
-  <si>
-    <t>997040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Firstname </t>
-  </si>
-  <si>
-    <t>Lastname</t>
-  </si>
-  <si>
-    <t>Options</t>
-  </si>
-  <si>
-    <t>Shane</t>
-  </si>
-  <si>
-    <t>Ward</t>
-  </si>
-  <si>
-    <t>TC_00_Login_OrangeHRM</t>
-  </si>
-  <si>
-    <t>Sagar</t>
-  </si>
-  <si>
-    <t>Test@123</t>
-  </si>
-  <si>
-    <t>Demo123</t>
-  </si>
-  <si>
-    <t>Test456</t>
+    <t>Adella</t>
+  </si>
+  <si>
+    <t>abcd@123</t>
+  </si>
+  <si>
+    <t>alice</t>
+  </si>
+  <si>
+    <t>amadi.aswad</t>
+  </si>
+  <si>
+    <t>andrew</t>
   </si>
 </sst>
 </file>
@@ -636,7 +645,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -650,13 +659,13 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -664,13 +673,13 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -678,13 +687,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
         <v>61</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -698,10 +707,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,7 +731,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -731,19 +740,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
         <v>54</v>
-      </c>
-      <c r="J1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -754,22 +763,22 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s">
         <v>47</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -780,18 +789,36 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{A23C96A3-FCA4-4943-A1C4-0CA95BAF5C57}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{1D74C58C-42E5-4527-843A-7E30F5582509}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -799,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,40 +861,40 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="K1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="Q1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -884,41 +911,41 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="Q2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -929,7 +956,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
@@ -947,7 +974,7 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -958,10 +985,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>64</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -984,13 +1011,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1012,10 +1039,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1038,10 +1065,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1065,9 +1092,10 @@
     <hyperlink ref="D7" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
     <hyperlink ref="C2" r:id="rId5" display="automation.catalogue@gmail.com" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
     <hyperlink ref="D2" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="D4" r:id="rId7" xr:uid="{FD38C22C-4859-4A53-B836-5703A466B471}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
RandomString and framework changes
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rehan\git\SeleniumLearning\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaradhyaVashisht\git\SeleniumLearning\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD79E36A-844A-4597-A3FD-5C59AB24F7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF123A8-D196-430A-8EE1-98E60F8E2D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRMLogin" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t>TC No</t>
   </si>
@@ -235,12 +235,31 @@
   </si>
   <si>
     <t>andrew</t>
+  </si>
+  <si>
+    <t>CHIFbM</t>
+  </si>
+  <si>
+    <t>LyuMwD</t>
+  </si>
+  <si>
+    <t>EjkKQUjc@gmail.com</t>
+  </si>
+  <si>
+    <t>tUzBQ</t>
+  </si>
+  <si>
+    <t>msSGx</t>
+  </si>
+  <si>
+    <t>fnnxoWnO@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -621,9 +640,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -709,18 +728,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -763,16 +782,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
         <v>36</v>
@@ -826,22 +845,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="22.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Changes made to test cases
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaradhyaVashisht\git\SeleniumLearning\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rehan\git\SeleniumLearning\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF123A8-D196-430A-8EE1-98E60F8E2D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D72178F-AFEC-4DFF-945C-B61793D514AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRMLogin" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
   <si>
     <t>TC No</t>
   </si>
@@ -78,18 +78,12 @@
     <t>6</t>
   </si>
   <si>
-    <t>Vijetha</t>
-  </si>
-  <si>
     <t>Admin@1234</t>
   </si>
   <si>
     <t>Hello@1235</t>
   </si>
   <si>
-    <t>Ravi</t>
-  </si>
-  <si>
     <t>Welcome@8907</t>
   </si>
   <si>
@@ -195,30 +189,9 @@
     <t>Options</t>
   </si>
   <si>
-    <t>Shane</t>
-  </si>
-  <si>
-    <t>Ward</t>
-  </si>
-  <si>
     <t>TC_00_Login_OrangeHRM</t>
   </si>
   <si>
-    <t>Sagar</t>
-  </si>
-  <si>
-    <t>Test@123</t>
-  </si>
-  <si>
-    <t>Demo123</t>
-  </si>
-  <si>
-    <t>Test456</t>
-  </si>
-  <si>
-    <t>log-in1234@gmail.com</t>
-  </si>
-  <si>
     <t>log-in123@gmail.com</t>
   </si>
   <si>
@@ -237,22 +210,40 @@
     <t>andrew</t>
   </si>
   <si>
-    <t>CHIFbM</t>
-  </si>
-  <si>
-    <t>LyuMwD</t>
-  </si>
-  <si>
-    <t>EjkKQUjc@gmail.com</t>
-  </si>
-  <si>
-    <t>tUzBQ</t>
-  </si>
-  <si>
-    <t>msSGx</t>
-  </si>
-  <si>
-    <t>fnnxoWnO@gmail.com</t>
+    <t>DtdUGL</t>
+  </si>
+  <si>
+    <t>mSfieX</t>
+  </si>
+  <si>
+    <t>IMIKFhCl@gmail.com</t>
+  </si>
+  <si>
+    <t>bBEcE</t>
+  </si>
+  <si>
+    <t>UEaWel</t>
+  </si>
+  <si>
+    <t>bsGpqnDXI@gmail.com</t>
+  </si>
+  <si>
+    <t>NUplY</t>
+  </si>
+  <si>
+    <t>DPApg</t>
+  </si>
+  <si>
+    <t>TTCmBkzf@gmail.com</t>
+  </si>
+  <si>
+    <t>OgkHG</t>
+  </si>
+  <si>
+    <t>opFVQ</t>
+  </si>
+  <si>
+    <t>GwiDFrKoK@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -634,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A749B9C4-BA88-4871-B800-71E148BFFD52}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -664,7 +655,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -678,13 +669,13 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -692,13 +683,13 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>60</v>
+        <v>53</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -706,21 +697,24 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>61</v>
+      <c r="D5" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{BED2620E-74FB-4FCC-8DE4-3F684ABB0AAE}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{CD8EF335-5DCD-4938-BF53-3FAF30ECE3B7}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{3F9A2B1E-E40F-4EBB-92A2-A0F3DA1BBBAD}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{AFB37B20-9363-475E-920D-B3A15023C072}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{4EB47153-C235-46BD-B7F3-5541C6539BF0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -728,7 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -750,7 +744,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -759,19 +753,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" t="s">
         <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -782,22 +776,22 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -808,13 +802,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -825,10 +819,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -846,7 +840,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,40 +874,40 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="N1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="P1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Q1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -930,41 +924,41 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="M2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -975,7 +969,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
@@ -993,7 +987,7 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -1004,10 +998,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1030,13 +1024,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1058,10 +1052,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1084,10 +1078,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>

</xml_diff>

<commit_message>
completed add employee test case
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,24 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rehan\git\SeleniumLearning\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D72178F-AFEC-4DFF-945C-B61793D514AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5241756E-E624-4765-A261-324820F32AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRMLogin" sheetId="4" r:id="rId1"/>
-    <sheet name="DemoWebShop" sheetId="1" r:id="rId2"/>
-    <sheet name="OrangeHRM" sheetId="2" r:id="rId3"/>
-    <sheet name="airbnb" sheetId="3" r:id="rId4"/>
+    <sheet name="DemoWebShopLogin" sheetId="5" r:id="rId2"/>
+    <sheet name="DemoWebShop" sheetId="1" r:id="rId3"/>
+    <sheet name="OrangeHRM" sheetId="2" r:id="rId4"/>
+    <sheet name="airbnb" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="61">
   <si>
     <t>TC No</t>
   </si>
@@ -81,12 +82,6 @@
     <t>Admin@1234</t>
   </si>
   <si>
-    <t>Hello@1235</t>
-  </si>
-  <si>
-    <t>Welcome@8907</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -204,53 +199,25 @@
     <t>alice</t>
   </si>
   <si>
-    <t>amadi.aswad</t>
-  </si>
-  <si>
-    <t>andrew</t>
-  </si>
-  <si>
-    <t>DtdUGL</t>
-  </si>
-  <si>
-    <t>mSfieX</t>
-  </si>
-  <si>
-    <t>IMIKFhCl@gmail.com</t>
-  </si>
-  <si>
-    <t>bBEcE</t>
-  </si>
-  <si>
-    <t>UEaWel</t>
-  </si>
-  <si>
-    <t>bsGpqnDXI@gmail.com</t>
-  </si>
-  <si>
-    <t>NUplY</t>
-  </si>
-  <si>
-    <t>DPApg</t>
-  </si>
-  <si>
-    <t>TTCmBkzf@gmail.com</t>
-  </si>
-  <si>
-    <t>OgkHG</t>
-  </si>
-  <si>
-    <t>opFVQ</t>
-  </si>
-  <si>
     <t>GwiDFrKoK@gmail.com</t>
+  </si>
+  <si>
+    <t>KmKwo</t>
+  </si>
+  <si>
+    <t>QCLQjr</t>
+  </si>
+  <si>
+    <t>XmwVSw</t>
+  </si>
+  <si>
+    <t>RxYEuAdru@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -625,15 +592,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A749B9C4-BA88-4871-B800-71E148BFFD52}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.6640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -655,7 +622,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -669,10 +636,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
@@ -683,13 +650,13 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -697,10 +664,10 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>16</v>
@@ -719,21 +686,116 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8611F935-D4B5-4EF5-9029-F2A425E632E8}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{9ADCE113-17A8-4A15-A379-DCDA05083A6A}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{7D3EA212-58B3-4B89-8DE0-2DE5512FEE37}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{1A91A12A-4022-4F42-ACED-540A47247392}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -744,7 +806,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -753,19 +815,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
         <v>50</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -776,22 +838,22 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -802,13 +864,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -819,10 +881,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -835,26 +897,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.44140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="19.33203125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="22.109375" collapsed="true"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -874,40 +936,40 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="N1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="P1" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Q1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -924,41 +986,41 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="M2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Q2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -969,7 +1031,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
@@ -987,7 +1049,7 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -998,10 +1060,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1024,13 +1086,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1051,17 +1113,19 @@
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="4"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -1077,12 +1141,8 @@
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="4"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1101,18 +1161,16 @@
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
     <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="D6" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="D7" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="C2" r:id="rId5" display="automation.catalogue@gmail.com" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="D2" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="D4" r:id="rId7" xr:uid="{FD38C22C-4859-4A53-B836-5703A466B471}"/>
+    <hyperlink ref="C2" r:id="rId3" display="automation.catalogue@gmail.com" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{FD38C22C-4859-4A53-B836-5703A466B471}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
TestNG Listeners are added
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="90">
   <si>
     <t>TC No</t>
   </si>
@@ -293,6 +293,12 @@
   </si>
   <si>
     <t>zTCcdEBrO@gmail.com</t>
+  </si>
+  <si>
+    <t>zJkBSyT</t>
+  </si>
+  <si>
+    <t>zxZYll</t>
   </si>
 </sst>
 </file>
@@ -1199,14 +1205,14 @@
       <c r="D6" s="4"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>

</xml_diff>

<commit_message>
Maven surefire plugin configured
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="105">
   <si>
     <t>TC No</t>
   </si>
@@ -299,6 +299,51 @@
   </si>
   <si>
     <t>zxZYll</t>
+  </si>
+  <si>
+    <t>sOXFr</t>
+  </si>
+  <si>
+    <t>veWKU</t>
+  </si>
+  <si>
+    <t>mPTlPZXUv@gmail.com</t>
+  </si>
+  <si>
+    <t>eGKtOu</t>
+  </si>
+  <si>
+    <t>ZYOHIj</t>
+  </si>
+  <si>
+    <t>fGMdAIfri@gmail.com</t>
+  </si>
+  <si>
+    <t>hNRUPc</t>
+  </si>
+  <si>
+    <t>faTOtX</t>
+  </si>
+  <si>
+    <t>ZCVcGlGfL@gmail.com</t>
+  </si>
+  <si>
+    <t>WhREE</t>
+  </si>
+  <si>
+    <t>iwCjd</t>
+  </si>
+  <si>
+    <t>QjGxRicSn@gmail.com</t>
+  </si>
+  <si>
+    <t>GkVWM</t>
+  </si>
+  <si>
+    <t>dIqyl</t>
+  </si>
+  <si>
+    <t>yYWfVclu@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -926,16 +971,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="H2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Changes in testcases architecture
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="114">
   <si>
     <t>TC No</t>
   </si>
@@ -344,6 +344,33 @@
   </si>
   <si>
     <t>yYWfVclu@gmail.com</t>
+  </si>
+  <si>
+    <t>yCyyJZ</t>
+  </si>
+  <si>
+    <t>pvAGLu</t>
+  </si>
+  <si>
+    <t>EgqHsuQN@gmail.com</t>
+  </si>
+  <si>
+    <t>iWVInI</t>
+  </si>
+  <si>
+    <t>GaPMVO</t>
+  </si>
+  <si>
+    <t>KlRNUIvH@gmail.com</t>
+  </si>
+  <si>
+    <t>XaXzmD</t>
+  </si>
+  <si>
+    <t>CFycbe</t>
+  </si>
+  <si>
+    <t>CGcZNtrtt@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -971,16 +998,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="G2" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="H2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Latest changes in framework
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="163">
   <si>
     <t>TC No</t>
   </si>
@@ -371,6 +371,153 @@
   </si>
   <si>
     <t>CGcZNtrtt@gmail.com</t>
+  </si>
+  <si>
+    <t>mSEYse</t>
+  </si>
+  <si>
+    <t>eVRhcQ</t>
+  </si>
+  <si>
+    <t>qJQnwkPIy@gmail.com</t>
+  </si>
+  <si>
+    <t>nzcBW</t>
+  </si>
+  <si>
+    <t>SzNsw</t>
+  </si>
+  <si>
+    <t>YfNXQNVA@gmail.com</t>
+  </si>
+  <si>
+    <t>fQcLHL</t>
+  </si>
+  <si>
+    <t>oSTkd</t>
+  </si>
+  <si>
+    <t>HTuAJEKO@gmail.com</t>
+  </si>
+  <si>
+    <t>lqggWO</t>
+  </si>
+  <si>
+    <t>aAFTm</t>
+  </si>
+  <si>
+    <t>CTxTWCCOb@gmail.com</t>
+  </si>
+  <si>
+    <t>anXPN</t>
+  </si>
+  <si>
+    <t>aCvQEx</t>
+  </si>
+  <si>
+    <t>BacgxriI@gmail.com</t>
+  </si>
+  <si>
+    <t>YOicS</t>
+  </si>
+  <si>
+    <t>juuOoP</t>
+  </si>
+  <si>
+    <t>hoVSLuXz@gmail.com</t>
+  </si>
+  <si>
+    <t>HdaPd</t>
+  </si>
+  <si>
+    <t>naPSnP</t>
+  </si>
+  <si>
+    <t>NKFNMGBGs@gmail.com</t>
+  </si>
+  <si>
+    <t>iDxTb</t>
+  </si>
+  <si>
+    <t>VBSHt</t>
+  </si>
+  <si>
+    <t>wcpaETrH@gmail.com</t>
+  </si>
+  <si>
+    <t>CdEyDq</t>
+  </si>
+  <si>
+    <t>LLaNth</t>
+  </si>
+  <si>
+    <t>WFByHLyJr@gmail.com</t>
+  </si>
+  <si>
+    <t>HdNtOj</t>
+  </si>
+  <si>
+    <t>hOqtKl</t>
+  </si>
+  <si>
+    <t>mmRVYLAE@gmail.com</t>
+  </si>
+  <si>
+    <t>ukfrU</t>
+  </si>
+  <si>
+    <t>FSNIGj</t>
+  </si>
+  <si>
+    <t>HroGVLEk@gmail.com</t>
+  </si>
+  <si>
+    <t>FYtNld</t>
+  </si>
+  <si>
+    <t>ZSPWXp</t>
+  </si>
+  <si>
+    <t>bXHFXMQXC@gmail.com</t>
+  </si>
+  <si>
+    <t>CPiQmm</t>
+  </si>
+  <si>
+    <t>PuEkKY</t>
+  </si>
+  <si>
+    <t>gNfEctwDF@gmail.com</t>
+  </si>
+  <si>
+    <t>thyRXv</t>
+  </si>
+  <si>
+    <t>cAkrYu</t>
+  </si>
+  <si>
+    <t>rtzrl</t>
+  </si>
+  <si>
+    <t>dUIMmrqL@gmail.com</t>
+  </si>
+  <si>
+    <t>vWbFZR</t>
+  </si>
+  <si>
+    <t>ldvjl</t>
+  </si>
+  <si>
+    <t>NOSdYrrtT@gmail.com</t>
+  </si>
+  <si>
+    <t>BhoUpu</t>
+  </si>
+  <si>
+    <t>rSWvWf</t>
+  </si>
+  <si>
+    <t>cYqcqcYb@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -998,16 +1145,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="G2" t="s">
-        <v>112</v>
+        <v>161</v>
       </c>
       <c r="H2" t="s">
         <v>32</v>
@@ -1277,14 +1424,14 @@
       <c r="D6" s="4"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>

</xml_diff>